<commit_message>
Added entity types and stuff
</commit_message>
<xml_diff>
--- a/DMDD/Casus/Feiten MSS.xlsx
+++ b/DMDD/Casus/Feiten MSS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\Han\ISE\DMDD\Casus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE936A2-08AF-4B39-B6D5-0C224157AFBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD61115-F253-464B-B5F2-E9B01732D828}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="170">
   <si>
     <t xml:space="preserve">Invoice </t>
   </si>
@@ -166,29 +166,387 @@
     <t>ET: Product</t>
   </si>
   <si>
-    <t>Het product</t>
-  </si>
-  <si>
-    <t>is een</t>
-  </si>
-  <si>
     <t>module</t>
   </si>
   <si>
-    <t>'</t>
-  </si>
-  <si>
     <t>case</t>
+  </si>
+  <si>
+    <t>Invoice No</t>
+  </si>
+  <si>
+    <t>was made on date</t>
+  </si>
+  <si>
+    <t>FT1:</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>is described as</t>
+  </si>
+  <si>
+    <t>Doepfer Low Cost Case 1 Row</t>
+  </si>
+  <si>
+    <t>Doepfer Low Cost Case 2 Row</t>
+  </si>
+  <si>
+    <t>has purchased a number of</t>
+  </si>
+  <si>
+    <t>of product</t>
+  </si>
+  <si>
+    <t>FT2:</t>
+  </si>
+  <si>
+    <t>FT4:</t>
+  </si>
+  <si>
+    <t>FT5:</t>
+  </si>
+  <si>
+    <t>is called</t>
+  </si>
+  <si>
+    <t>Doepfer Low Cost Case 3 Row</t>
+  </si>
+  <si>
+    <t>FT6:</t>
+  </si>
+  <si>
+    <t>1499083-89</t>
+  </si>
+  <si>
+    <t>has a Product Variant</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>1499083-90</t>
+  </si>
+  <si>
+    <t>1499083-91</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>FT7:</t>
+  </si>
+  <si>
+    <t>is of Product type</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>FT8:</t>
+  </si>
+  <si>
+    <t>The Doepfer Low Cost Case 2 Rows is a…</t>
+  </si>
+  <si>
+    <t>The Doepfer Low Cost Case 3 Rows is a…</t>
+  </si>
+  <si>
+    <t>The Doepfer Low Cost Case 1 Row is a…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1380b </t>
+  </si>
+  <si>
+    <t>currently has a purchasing price of</t>
+  </si>
+  <si>
+    <t>FT9:</t>
+  </si>
+  <si>
+    <t>currently has a selling price of</t>
+  </si>
+  <si>
+    <t>FT10:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product </t>
+  </si>
+  <si>
+    <t>is manufactured by</t>
+  </si>
+  <si>
+    <t>FT11:</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Doepfer Gmbh</t>
+  </si>
+  <si>
+    <t>is based in</t>
+  </si>
+  <si>
+    <t>Ljunggren Audio</t>
+  </si>
+  <si>
+    <t>Smorbord</t>
+  </si>
+  <si>
+    <t>Royal Ohm</t>
+  </si>
+  <si>
+    <t>MFB GmbH</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>FT12:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'s address is </t>
+  </si>
+  <si>
+    <t>Becksjudarvägen 4A</t>
+  </si>
+  <si>
+    <t>Marconistrasse 24</t>
+  </si>
+  <si>
+    <t>FT16:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer </t>
+  </si>
+  <si>
+    <t>Doepfer GmbH’s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ZIP code is</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D-82166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "            " </t>
+  </si>
+  <si>
+    <t xml:space="preserve">660 64 </t>
+  </si>
+  <si>
+    <t>FT17:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can be reached via phone on </t>
+  </si>
+  <si>
+    <t>+49 89 89809510</t>
+  </si>
+  <si>
+    <t>011-46-98-012-345</t>
+  </si>
+  <si>
+    <t>+66 38 517 332</t>
+  </si>
+  <si>
+    <t>FT18:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can be reached via email on  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@ljunggrenaudio.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">export@royalohm.com </t>
+  </si>
+  <si>
+    <t>FT19:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starter Set </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doepfer 3 Row Starter Set </t>
+  </si>
+  <si>
+    <t>contains product</t>
+  </si>
+  <si>
+    <t>A-100LC9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doepfer 4 Row Starter Set </t>
+  </si>
+  <si>
+    <t>A-100LC10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doepfer 5 Row Starter Set </t>
+  </si>
+  <si>
+    <t>A-100LC11</t>
+  </si>
+  <si>
+    <t>FT20:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provides space for </t>
+  </si>
+  <si>
+    <t>FT21:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Of product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there are </t>
+  </si>
+  <si>
+    <t>FT23:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patch Cable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-100C30 </t>
+  </si>
+  <si>
+    <t>A-100C50</t>
+  </si>
+  <si>
+    <t>A-100C70</t>
+  </si>
+  <si>
+    <t>FT24:</t>
+  </si>
+  <si>
+    <t>with a product note</t>
+  </si>
+  <si>
+    <t>Full DIY Kit</t>
+  </si>
+  <si>
+    <t>PCB Only Kit</t>
+  </si>
+  <si>
+    <t>Pre-Build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doepfer Low cost case 1 row </t>
+  </si>
+  <si>
+    <t>Doepfer Low cost case 2 rows</t>
+  </si>
+  <si>
+    <t>Doepfer Low cost case 3 rows</t>
+  </si>
+  <si>
+    <t>ET: Invoice</t>
+  </si>
+  <si>
+    <t>ATT: Date</t>
+  </si>
+  <si>
+    <t>ID: ATT Invoice_No</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>ATT: Quantity</t>
+  </si>
+  <si>
+    <t>ID: Att Product_Code</t>
+  </si>
+  <si>
+    <t>ATT: Product_Name</t>
+  </si>
+  <si>
+    <t>ATT: Product_Variant</t>
+  </si>
+  <si>
+    <t>ATT: Product_Type</t>
+  </si>
+  <si>
+    <t>ATT: Product_Description</t>
+  </si>
+  <si>
+    <t>ATT: Purchasing_Price</t>
+  </si>
+  <si>
+    <t>ATT: Selling_Price</t>
+  </si>
+  <si>
+    <t>ET: Manufacturer</t>
+  </si>
+  <si>
+    <t>ID: Att Manufacturer_name</t>
+  </si>
+  <si>
+    <t>ATT: City</t>
+  </si>
+  <si>
+    <t>ATT: Address</t>
+  </si>
+  <si>
+    <t>ATT: ZIP_Code</t>
+  </si>
+  <si>
+    <t>ATT: Phone_No</t>
+  </si>
+  <si>
+    <t>ATT: Email</t>
+  </si>
+  <si>
+    <t>in stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 centimeters </t>
+  </si>
+  <si>
+    <t>in length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 centimeters </t>
+  </si>
+  <si>
+    <t>70 centimeters</t>
+  </si>
+  <si>
+    <t>row of modules</t>
+  </si>
+  <si>
+    <t>ATT: Number_Of_Modules</t>
+  </si>
+  <si>
+    <t>ATT: Stock</t>
+  </si>
+  <si>
+    <t>ATT: Cable_Length</t>
+  </si>
+  <si>
+    <t>ATT:Product_Note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +564,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,11 +680,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -404,15 +777,105 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1485,53 +1948,1970 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD2064A-CA15-4720-B0DF-1590FE7B2FF0}">
-  <dimension ref="C4:F6"/>
+  <dimension ref="B3:K173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="59">
+        <v>160154</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="60">
+        <v>43427</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="59">
+        <v>160155</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="60">
+        <v>43428</v>
+      </c>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="66">
+        <v>160156</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="67">
+        <v>43429</v>
+      </c>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="59"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+    </row>
+    <row r="9" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="61"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+    </row>
+    <row r="10" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="61"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+    </row>
+    <row r="11" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="61"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="62">
+        <v>160154</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="64">
+        <v>1</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="62">
+        <v>160155</v>
+      </c>
+      <c r="E14" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="64">
+        <v>2</v>
+      </c>
+      <c r="G14" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="68">
+        <v>160156</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="69">
+        <v>3</v>
+      </c>
+      <c r="G15" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="55"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="55"/>
+    </row>
+    <row r="17" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="55"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="I17" s="55"/>
+    </row>
+    <row r="18" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="62"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+    </row>
+    <row r="19" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="62"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+    </row>
+    <row r="20" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="62"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="42"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="71" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="42"/>
+    </row>
+    <row r="28" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="42"/>
+    </row>
+    <row r="29" spans="2:9" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="42"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="42"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="72" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="42"/>
+    </row>
+    <row r="37" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="42"/>
+    </row>
+    <row r="38" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="42"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="42"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="42">
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="42"/>
+    </row>
+    <row r="46" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="42"/>
+    </row>
+    <row r="47" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="42"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="43"/>
+    </row>
+    <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C49" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C50" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C51" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" s="73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" s="47">
+        <v>180.95</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="47">
+        <v>181.95</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="75">
+        <v>182.95</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>51</v>
+      </c>
+      <c r="D67" t="s">
+        <v>77</v>
+      </c>
+      <c r="E67" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" s="47">
+        <v>249.99</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="47">
+        <v>250.99</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F69" s="75">
+        <v>251.99</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" t="s">
+        <v>77</v>
+      </c>
+      <c r="E76" t="s">
+        <v>83</v>
+      </c>
+      <c r="F76" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>3</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C78" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>3</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C79" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" s="72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="F80" s="72" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>85</v>
+      </c>
+      <c r="D85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E85" t="s">
+        <v>87</v>
+      </c>
+      <c r="F85" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>88</v>
+      </c>
+      <c r="E86" t="s">
+        <v>3</v>
+      </c>
+      <c r="F86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C87" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" t="s">
+        <v>3</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C88" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F88" s="72" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="2:6" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="F94" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>88</v>
+      </c>
+      <c r="E95" t="s">
+        <v>3</v>
+      </c>
+      <c r="F95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C96" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C97" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F97" s="72" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C98" s="72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B102" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D102" s="53"/>
+      <c r="E102" s="53"/>
+      <c r="F102" s="53"/>
+      <c r="G102" s="53"/>
+      <c r="H102" s="53"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B103" s="45"/>
+      <c r="C103" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D103" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E103" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="G103" s="55"/>
+      <c r="H103" s="55"/>
+      <c r="I103" s="55"/>
+      <c r="J103" s="55"/>
+      <c r="K103" s="55"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B104" s="45"/>
+      <c r="C104" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D104" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E104" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F104" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="G104" s="55"/>
+      <c r="H104" s="55"/>
+      <c r="I104" s="55"/>
+      <c r="J104" s="55"/>
+      <c r="K104" s="55"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B105" s="45"/>
+      <c r="C105" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D105" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E105" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F105" s="76">
+        <v>24000</v>
+      </c>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="55"/>
+      <c r="J105" s="55"/>
+      <c r="K105" s="55"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B106" s="45"/>
+      <c r="C106" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D106" s="55"/>
+      <c r="E106" s="55"/>
+      <c r="F106" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="G106" s="55"/>
+      <c r="H106" s="55"/>
+      <c r="I106" s="55"/>
+      <c r="J106" s="55"/>
+      <c r="K106" s="55"/>
+    </row>
+    <row r="107" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="45"/>
+      <c r="C107" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="D107" s="55"/>
+      <c r="E107" s="55"/>
+      <c r="F107" s="55"/>
+      <c r="G107" s="55"/>
+      <c r="H107" s="55"/>
+      <c r="I107" s="55"/>
+      <c r="J107" s="55"/>
+      <c r="K107" s="55"/>
+    </row>
+    <row r="108" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="45"/>
+      <c r="C108" s="55"/>
+      <c r="D108" s="55"/>
+      <c r="E108" s="55"/>
+      <c r="F108" s="55"/>
+      <c r="G108" s="55"/>
+      <c r="H108" s="55"/>
+      <c r="I108" s="55"/>
+      <c r="J108" s="55"/>
+      <c r="K108" s="55"/>
+    </row>
+    <row r="109" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="45"/>
+      <c r="C109" s="55"/>
+      <c r="D109" s="55"/>
+      <c r="E109" s="55"/>
+      <c r="F109" s="55"/>
+      <c r="G109" s="55"/>
+      <c r="H109" s="55"/>
+      <c r="I109" s="55"/>
+      <c r="J109" s="55"/>
+      <c r="K109" s="55"/>
+    </row>
+    <row r="110" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="45"/>
+      <c r="C110" s="55"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="55"/>
+      <c r="F110" s="55"/>
+      <c r="G110" s="55"/>
+      <c r="H110" s="55"/>
+      <c r="I110" s="55"/>
+      <c r="J110" s="55"/>
+      <c r="K110" s="55"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B111" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C111" s="55"/>
+      <c r="D111" s="55"/>
+      <c r="E111" s="55"/>
+      <c r="F111" s="55"/>
+      <c r="G111" s="55"/>
+      <c r="H111" s="55"/>
+      <c r="I111" s="55"/>
+      <c r="J111" s="55"/>
+      <c r="K111" s="55"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B112" s="45"/>
+      <c r="C112" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D112" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E112" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="F112" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="G112" s="55"/>
+      <c r="H112" s="55"/>
+      <c r="I112" s="55"/>
+      <c r="J112" s="55"/>
+      <c r="K112" s="55"/>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B113" s="45"/>
+      <c r="C113" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D113" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E113" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F113" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="G113" s="55"/>
+      <c r="H113" s="55"/>
+      <c r="I113" s="55"/>
+      <c r="J113" s="55"/>
+      <c r="K113" s="55"/>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B114" s="45"/>
+      <c r="C114" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D114" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E114" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F114" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="G114" s="55"/>
+      <c r="H114" s="55"/>
+      <c r="I114" s="55"/>
+      <c r="J114" s="55"/>
+      <c r="K114" s="55"/>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B115" s="45"/>
+      <c r="C115" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D115" s="55"/>
+      <c r="E115" s="55"/>
+      <c r="F115" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="G115" s="55"/>
+      <c r="H115" s="55"/>
+      <c r="I115" s="55"/>
+      <c r="J115" s="55"/>
+      <c r="K115" s="55"/>
+    </row>
+    <row r="116" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="45"/>
+      <c r="C116" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="D116" s="55"/>
+      <c r="E116" s="55"/>
+      <c r="F116" s="55"/>
+      <c r="G116" s="55"/>
+      <c r="H116" s="55"/>
+      <c r="I116" s="55"/>
+      <c r="J116" s="55"/>
+      <c r="K116" s="55"/>
+    </row>
+    <row r="117" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="45"/>
+      <c r="C117" s="55"/>
+      <c r="D117" s="55"/>
+      <c r="E117" s="55"/>
+      <c r="F117" s="55"/>
+      <c r="G117" s="55"/>
+      <c r="H117" s="55"/>
+      <c r="I117" s="55"/>
+      <c r="J117" s="55"/>
+      <c r="K117" s="55"/>
+    </row>
+    <row r="118" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="45"/>
+      <c r="C118" s="55"/>
+      <c r="D118" s="55"/>
+      <c r="E118" s="55"/>
+      <c r="F118" s="55"/>
+      <c r="G118" s="55"/>
+      <c r="H118" s="55"/>
+      <c r="I118" s="55"/>
+      <c r="J118" s="55"/>
+      <c r="K118" s="55"/>
+    </row>
+    <row r="119" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="45"/>
+      <c r="C119" s="55"/>
+      <c r="D119" s="55"/>
+      <c r="E119" s="55"/>
+      <c r="F119" s="55"/>
+      <c r="G119" s="55"/>
+      <c r="H119" s="55"/>
+      <c r="I119" s="55"/>
+      <c r="J119" s="55"/>
+      <c r="K119" s="55"/>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B120" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C120" s="55"/>
+      <c r="D120" s="55"/>
+      <c r="E120" s="55"/>
+      <c r="F120" s="55"/>
+      <c r="G120" s="55"/>
+      <c r="H120" s="55"/>
+      <c r="I120" s="55"/>
+      <c r="J120" s="55"/>
+      <c r="K120" s="55"/>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B121" s="45"/>
+      <c r="C121" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D121" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E121" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F121" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="G121" s="55"/>
+      <c r="H121" s="55"/>
+      <c r="I121" s="55"/>
+      <c r="J121" s="55"/>
+      <c r="K121" s="55"/>
+    </row>
+    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B122" s="45"/>
+      <c r="C122" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D122" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E122" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F122" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="G122" s="55"/>
+      <c r="H122" s="55"/>
+      <c r="I122" s="55"/>
+      <c r="J122" s="55"/>
+      <c r="K122" s="55"/>
+    </row>
+    <row r="123" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B123" s="45"/>
+      <c r="C123" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D123" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E123" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F123" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="G123" s="55"/>
+      <c r="H123" s="55"/>
+      <c r="I123" s="55"/>
+      <c r="J123" s="55"/>
+      <c r="K123" s="55"/>
+    </row>
+    <row r="124" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B124" s="45"/>
+      <c r="C124" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="55"/>
+      <c r="E124" s="55"/>
+      <c r="F124" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="G124" s="55"/>
+      <c r="H124" s="55"/>
+      <c r="I124" s="55"/>
+      <c r="J124" s="55"/>
+      <c r="K124" s="55"/>
+    </row>
+    <row r="125" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="45"/>
+      <c r="C125" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="D125" s="55"/>
+      <c r="E125" s="55"/>
+      <c r="F125" s="55"/>
+      <c r="G125" s="55"/>
+      <c r="H125" s="55"/>
+      <c r="I125" s="55"/>
+      <c r="J125" s="55"/>
+      <c r="K125" s="55"/>
+    </row>
+    <row r="126" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="45"/>
+      <c r="C126" s="55"/>
+      <c r="D126" s="55"/>
+      <c r="E126" s="55"/>
+      <c r="F126" s="55"/>
+      <c r="G126" s="55"/>
+      <c r="H126" s="55"/>
+      <c r="I126" s="55"/>
+      <c r="J126" s="55"/>
+      <c r="K126" s="55"/>
+    </row>
+    <row r="127" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="45"/>
+      <c r="C127" s="55"/>
+      <c r="D127" s="55"/>
+      <c r="E127" s="55"/>
+      <c r="F127" s="55"/>
+      <c r="G127" s="55"/>
+      <c r="H127" s="55"/>
+      <c r="I127" s="55"/>
+      <c r="J127" s="55"/>
+      <c r="K127" s="55"/>
+    </row>
+    <row r="128" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="45"/>
+      <c r="C128" s="55"/>
+      <c r="D128" s="55"/>
+      <c r="E128" s="55"/>
+      <c r="F128" s="55"/>
+      <c r="G128" s="55"/>
+      <c r="H128" s="55"/>
+      <c r="I128" s="55"/>
+      <c r="J128" s="55"/>
+      <c r="K128" s="55"/>
+    </row>
+    <row r="129" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B129" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C129" s="55"/>
+      <c r="D129" s="55"/>
+      <c r="E129" s="55"/>
+      <c r="F129" s="55"/>
+      <c r="G129" s="55"/>
+      <c r="H129" s="55"/>
+      <c r="I129" s="55"/>
+      <c r="J129" s="55"/>
+      <c r="K129" s="55"/>
+    </row>
+    <row r="130" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B130" s="45"/>
+      <c r="C130" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D130" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E130" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="F130" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G130" s="55"/>
+      <c r="H130" s="55"/>
+      <c r="I130" s="55"/>
+      <c r="J130" s="55"/>
+      <c r="K130" s="55"/>
+    </row>
+    <row r="131" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B131" s="45"/>
+      <c r="C131" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D131" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E131" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F131" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="G131" s="55"/>
+      <c r="H131" s="55"/>
+      <c r="I131" s="55"/>
+      <c r="J131" s="55"/>
+      <c r="K131" s="55"/>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B132" s="45"/>
+      <c r="C132" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D132" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="E132" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F132" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="G132" s="55"/>
+      <c r="H132" s="55"/>
+      <c r="I132" s="55"/>
+      <c r="J132" s="55"/>
+      <c r="K132" s="55"/>
+    </row>
+    <row r="133" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B133" s="45"/>
+      <c r="C133" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D133" s="55"/>
+      <c r="E133" s="55"/>
+      <c r="F133" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="G133" s="55"/>
+      <c r="H133" s="55"/>
+      <c r="I133" s="55"/>
+      <c r="J133" s="55"/>
+      <c r="K133" s="55"/>
+    </row>
+    <row r="134" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="45"/>
+      <c r="C134" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D134" s="55"/>
+      <c r="E134" s="55"/>
+      <c r="F134" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="G134" s="55"/>
+      <c r="H134" s="55"/>
+      <c r="I134" s="55"/>
+      <c r="J134" s="55"/>
+      <c r="K134" s="55"/>
+    </row>
+    <row r="135" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="45"/>
+      <c r="C135" s="55"/>
+      <c r="D135" s="55"/>
+      <c r="E135" s="55"/>
+      <c r="F135" s="55"/>
+      <c r="G135" s="55"/>
+      <c r="H135" s="55"/>
+      <c r="I135" s="55"/>
+      <c r="J135" s="55"/>
+      <c r="K135" s="55"/>
+    </row>
+    <row r="136" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="45"/>
+      <c r="C136" s="55"/>
+      <c r="D136" s="55"/>
+      <c r="E136" s="55"/>
+      <c r="F136" s="55"/>
+      <c r="G136" s="55"/>
+      <c r="H136" s="55"/>
+      <c r="I136" s="55"/>
+      <c r="J136" s="55"/>
+      <c r="K136" s="55"/>
+    </row>
+    <row r="137" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="45"/>
+      <c r="C137" s="55"/>
+      <c r="D137" s="55"/>
+      <c r="E137" s="55"/>
+      <c r="F137" s="55"/>
+      <c r="G137" s="55"/>
+      <c r="H137" s="55"/>
+      <c r="I137" s="55"/>
+      <c r="J137" s="55"/>
+      <c r="K137" s="55"/>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B138" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C138" s="55"/>
+      <c r="D138" s="55"/>
+      <c r="E138" s="55"/>
+      <c r="F138" s="55"/>
+      <c r="G138" s="55"/>
+      <c r="H138" s="55"/>
+      <c r="I138" s="55"/>
+      <c r="J138" s="55"/>
+      <c r="K138" s="55"/>
+    </row>
+    <row r="139" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B139" s="45"/>
+      <c r="C139" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="E139" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="F139" s="56">
         <v>1</v>
       </c>
-      <c r="E4" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="G139" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="H139" s="55"/>
+      <c r="I139" s="55"/>
+      <c r="J139" s="55"/>
+      <c r="K139" s="55"/>
+    </row>
+    <row r="140" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B140" s="45"/>
+      <c r="C140" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D140" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="E140" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F140" s="56">
         <v>2</v>
       </c>
-      <c r="E5" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="G140" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H140" s="55"/>
+      <c r="I140" s="55"/>
+      <c r="J140" s="55"/>
+      <c r="K140" s="55"/>
+    </row>
+    <row r="141" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B141" s="45"/>
+      <c r="C141" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D141" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E141" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F141" s="77">
+        <v>3</v>
+      </c>
+      <c r="G141" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H141" s="55"/>
+      <c r="I141" s="55"/>
+      <c r="J141" s="55"/>
+      <c r="K141" s="55"/>
+    </row>
+    <row r="142" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B142" s="45"/>
+      <c r="C142" s="55" t="s">
         <v>45</v>
       </c>
+      <c r="D142" s="55"/>
+      <c r="E142" s="55"/>
+      <c r="F142" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="G142" s="55"/>
+      <c r="H142" s="55"/>
+      <c r="I142" s="55"/>
+      <c r="J142" s="55"/>
+      <c r="K142" s="55"/>
+    </row>
+    <row r="143" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="45"/>
+      <c r="C143" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D143" s="55"/>
+      <c r="E143" s="55"/>
+      <c r="F143" s="55"/>
+      <c r="G143" s="55"/>
+      <c r="H143" s="55"/>
+      <c r="I143" s="55"/>
+      <c r="J143" s="55"/>
+      <c r="K143" s="55"/>
+    </row>
+    <row r="144" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="45"/>
+      <c r="C144" s="55"/>
+      <c r="D144" s="55"/>
+      <c r="E144" s="55"/>
+      <c r="F144" s="55"/>
+      <c r="G144" s="55"/>
+      <c r="H144" s="55"/>
+      <c r="I144" s="55"/>
+      <c r="J144" s="55"/>
+      <c r="K144" s="55"/>
+    </row>
+    <row r="145" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="45"/>
+      <c r="C145" s="55"/>
+      <c r="D145" s="55"/>
+      <c r="E145" s="55"/>
+      <c r="F145" s="55"/>
+      <c r="G145" s="55"/>
+      <c r="H145" s="55"/>
+      <c r="I145" s="55"/>
+      <c r="J145" s="55"/>
+      <c r="K145" s="55"/>
+    </row>
+    <row r="146" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="45"/>
+      <c r="C146" s="55"/>
+      <c r="D146" s="55"/>
+      <c r="E146" s="55"/>
+      <c r="F146" s="55"/>
+      <c r="G146" s="55"/>
+      <c r="H146" s="55"/>
+      <c r="I146" s="55"/>
+      <c r="J146" s="55"/>
+      <c r="K146" s="55"/>
+    </row>
+    <row r="147" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B147" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C147" s="55"/>
+      <c r="D147" s="55"/>
+      <c r="E147" s="55"/>
+      <c r="F147" s="55"/>
+      <c r="G147" s="55"/>
+      <c r="H147" s="55"/>
+      <c r="I147" s="55"/>
+      <c r="J147" s="55"/>
+      <c r="K147" s="55"/>
+    </row>
+    <row r="148" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B148" s="45"/>
+      <c r="C148" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D148" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E148" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="F148" s="56">
+        <v>20</v>
+      </c>
+      <c r="G148" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="H148" s="55"/>
+      <c r="I148" s="55"/>
+      <c r="J148" s="55"/>
+      <c r="K148" s="55"/>
+    </row>
+    <row r="149" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B149" s="45"/>
+      <c r="C149" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D149" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E149" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F149" s="56">
+        <v>10</v>
+      </c>
+      <c r="G149" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H149" s="55"/>
+      <c r="I149" s="55"/>
+      <c r="J149" s="55"/>
+      <c r="K149" s="55"/>
+    </row>
+    <row r="150" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B150" s="45"/>
+      <c r="C150" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D150" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F150" s="77">
+        <v>30</v>
+      </c>
+      <c r="G150" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H150" s="55"/>
+      <c r="I150" s="55"/>
+      <c r="J150" s="55"/>
+      <c r="K150" s="55"/>
+    </row>
+    <row r="151" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B151" s="45"/>
+      <c r="C151" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D151" s="55"/>
+      <c r="E151" s="55"/>
+      <c r="F151" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="G151" s="55"/>
+      <c r="H151" s="55"/>
+      <c r="I151" s="55"/>
+      <c r="J151" s="55"/>
+      <c r="K151" s="55"/>
+    </row>
+    <row r="152" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="45"/>
+      <c r="C152" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D152" s="55"/>
+      <c r="E152" s="55"/>
+      <c r="F152" s="55"/>
+      <c r="G152" s="55"/>
+      <c r="H152" s="55"/>
+      <c r="I152" s="55"/>
+      <c r="J152" s="55"/>
+      <c r="K152" s="55"/>
+    </row>
+    <row r="153" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="45"/>
+      <c r="C153" s="55"/>
+      <c r="D153" s="55"/>
+      <c r="E153" s="55"/>
+      <c r="F153" s="55"/>
+      <c r="G153" s="55"/>
+      <c r="H153" s="55"/>
+      <c r="I153" s="55"/>
+      <c r="J153" s="55"/>
+      <c r="K153" s="55"/>
+    </row>
+    <row r="154" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="45"/>
+      <c r="C154" s="55"/>
+      <c r="D154" s="55"/>
+      <c r="E154" s="55"/>
+      <c r="F154" s="55"/>
+      <c r="G154" s="55"/>
+      <c r="H154" s="55"/>
+      <c r="I154" s="55"/>
+      <c r="J154" s="55"/>
+      <c r="K154" s="55"/>
+    </row>
+    <row r="155" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="45"/>
+      <c r="C155" s="55"/>
+      <c r="D155" s="55"/>
+      <c r="E155" s="55"/>
+      <c r="F155" s="55"/>
+      <c r="G155" s="55"/>
+      <c r="H155" s="55"/>
+      <c r="I155" s="55"/>
+      <c r="J155" s="55"/>
+      <c r="K155" s="55"/>
+    </row>
+    <row r="156" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="45"/>
+      <c r="C156" s="55"/>
+      <c r="D156" s="55"/>
+      <c r="E156" s="55"/>
+      <c r="F156" s="55"/>
+      <c r="G156" s="55"/>
+      <c r="H156" s="55"/>
+      <c r="I156" s="55"/>
+      <c r="J156" s="55"/>
+      <c r="K156" s="55"/>
+    </row>
+    <row r="157" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="45"/>
+      <c r="C157" s="55"/>
+      <c r="D157" s="55"/>
+      <c r="E157" s="55"/>
+      <c r="F157" s="55"/>
+      <c r="G157" s="55"/>
+      <c r="H157" s="55"/>
+      <c r="I157" s="55"/>
+      <c r="J157" s="55"/>
+      <c r="K157" s="55"/>
+    </row>
+    <row r="158" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="45"/>
+      <c r="C158" s="55"/>
+      <c r="D158" s="55"/>
+      <c r="E158" s="55"/>
+      <c r="F158" s="55"/>
+      <c r="G158" s="55"/>
+      <c r="H158" s="55"/>
+      <c r="I158" s="55"/>
+      <c r="J158" s="55"/>
+      <c r="K158" s="55"/>
+    </row>
+    <row r="159" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B159" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C159" s="55"/>
+      <c r="D159" s="55"/>
+      <c r="E159" s="55"/>
+      <c r="F159" s="55"/>
+      <c r="G159" s="55"/>
+      <c r="H159" s="55"/>
+      <c r="I159" s="55"/>
+      <c r="J159" s="55"/>
+      <c r="K159" s="55"/>
+    </row>
+    <row r="160" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B160" s="45"/>
+      <c r="C160" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="D160" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="E160" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="F160" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="G160" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="H160" s="55"/>
+      <c r="I160" s="55"/>
+      <c r="J160" s="55"/>
+      <c r="K160" s="55"/>
+    </row>
+    <row r="161" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B161" s="45"/>
+      <c r="C161" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D161" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E161" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="F161" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="G161" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H161" s="55"/>
+      <c r="I161" s="55"/>
+      <c r="J161" s="55"/>
+      <c r="K161" s="55"/>
+    </row>
+    <row r="162" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B162" s="45"/>
+      <c r="C162" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D162" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="E162" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F162" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="G162" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H162" s="55"/>
+      <c r="I162" s="55"/>
+      <c r="J162" s="55"/>
+      <c r="K162" s="55"/>
+    </row>
+    <row r="163" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B163" s="45"/>
+      <c r="C163" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D163" s="55"/>
+      <c r="E163" s="55"/>
+      <c r="F163" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="G163" s="55"/>
+      <c r="H163" s="55"/>
+      <c r="I163" s="55"/>
+      <c r="J163" s="55"/>
+      <c r="K163" s="55"/>
+    </row>
+    <row r="164" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="45"/>
+      <c r="C164" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D164" s="55"/>
+      <c r="E164" s="55"/>
+      <c r="F164" s="55"/>
+      <c r="G164" s="55"/>
+      <c r="H164" s="55"/>
+      <c r="I164" s="55"/>
+      <c r="J164" s="55"/>
+      <c r="K164" s="55"/>
+    </row>
+    <row r="165" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="45"/>
+      <c r="C165" s="55"/>
+      <c r="D165" s="55"/>
+      <c r="E165" s="55"/>
+      <c r="F165" s="55"/>
+      <c r="G165" s="55"/>
+      <c r="H165" s="55"/>
+      <c r="I165" s="55"/>
+      <c r="J165" s="55"/>
+      <c r="K165" s="55"/>
+    </row>
+    <row r="166" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="45"/>
+      <c r="C166" s="55"/>
+      <c r="D166" s="55"/>
+      <c r="E166" s="55"/>
+      <c r="F166" s="55"/>
+      <c r="G166" s="55"/>
+      <c r="H166" s="55"/>
+      <c r="I166" s="55"/>
+      <c r="J166" s="55"/>
+      <c r="K166" s="55"/>
+    </row>
+    <row r="167" spans="2:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="45"/>
+      <c r="C167" s="55"/>
+      <c r="D167" s="55"/>
+      <c r="E167" s="55"/>
+      <c r="F167" s="55"/>
+      <c r="G167" s="55"/>
+      <c r="H167" s="55"/>
+      <c r="I167" s="55"/>
+      <c r="J167" s="55"/>
+      <c r="K167" s="55"/>
+    </row>
+    <row r="168" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B168" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C168" s="55"/>
+      <c r="D168" s="55"/>
+      <c r="E168" s="55"/>
+      <c r="F168" s="55"/>
+      <c r="G168" s="55"/>
+      <c r="H168" s="55"/>
+      <c r="I168" s="55"/>
+      <c r="J168" s="55"/>
+      <c r="K168" s="55"/>
+    </row>
+    <row r="169" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B169" s="45"/>
+      <c r="C169" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D169" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="E169" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F169" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="I169" s="55"/>
+      <c r="J169" s="55"/>
+      <c r="K169" s="55"/>
+    </row>
+    <row r="170" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B170" s="45"/>
+      <c r="C170" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D170" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E170" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F170" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="I170" s="55"/>
+      <c r="J170" s="55"/>
+      <c r="K170" s="55"/>
+    </row>
+    <row r="171" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B171" s="45"/>
+      <c r="C171" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D171" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="E171" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F171" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="I171" s="55"/>
+      <c r="J171" s="55"/>
+      <c r="K171" s="55"/>
+    </row>
+    <row r="172" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C172" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="F172" s="62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="173" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C173" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="F173" s="62"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F121" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F123" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F122" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aanpassingen aan verwoordingen en cdm
</commit_message>
<xml_diff>
--- a/DMDD/Casus/Feiten MSS.xlsx
+++ b/DMDD/Casus/Feiten MSS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\School\Han\ISE\DMDD\Casus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853D0EBC-387E-4D3A-AF1B-0CE78286B858}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F507AF54-0269-43E1-9C64-11AD930A9FB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1980,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD2064A-CA15-4720-B0DF-1590FE7B2FF0}">
   <dimension ref="B3:M177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I149" sqref="I149"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2459,7 +2459,7 @@
       <c r="E48"/>
       <c r="F48"/>
     </row>
-    <row r="49" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C49" s="50" t="s">
         <v>51</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C50" s="43" t="s">
         <v>3</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C51" s="70" t="s">
         <v>3</v>
       </c>
@@ -3972,13 +3972,13 @@
       <c r="D171" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="E171" s="59" t="s">
+      <c r="E171" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F171" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="G171" s="66" t="s">
+      <c r="G171" s="59" t="s">
         <v>102</v>
       </c>
       <c r="H171" s="66" t="s">

</xml_diff>